<commit_message>
update project to UE5
</commit_message>
<xml_diff>
--- a/Content/Tables/GameData.xlsx
+++ b/Content/Tables/GameData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B705514-7EF7-483F-AE09-2ABFBA22D370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A039AFDD-0726-4EBF-BD81-49C4555A235D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -391,7 +391,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C2">
         <v>30</v>

</xml_diff>